<commit_message>
stopping point before two fictitious
</commit_message>
<xml_diff>
--- a/conejo/formatted_data.xlsx
+++ b/conejo/formatted_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\pyComms\conejo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D9BB5-8CA0-44D3-927F-B93D35153C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6942DF3-E2AB-44A2-9EC7-8C7A84B76E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B2B3255C-86D4-4B94-9983-7EF4502B7862}"/>
+    <workbookView xWindow="11160" yWindow="1455" windowWidth="14850" windowHeight="10200" activeTab="2" xr2:uid="{B2B3255C-86D4-4B94-9983-7EF4502B7862}"/>
   </bookViews>
   <sheets>
     <sheet name="busses" sheetId="2" r:id="rId1"/>
@@ -1269,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FB4950-8AF2-4919-9162-03A3918F6395}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
@@ -3881,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE3EA53-F01C-4E2B-BB06-AD151A3AC232}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68:M100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8005,8 +8005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F8381-333D-427E-B2F5-663E2125B366}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="K121" sqref="K121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8575,7 +8575,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="K13">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="L13">
         <v>208</v>
@@ -9851,7 +9851,7 @@
         <v>0.155</v>
       </c>
       <c r="K42">
-        <v>24</v>
+        <v>500</v>
       </c>
       <c r="L42">
         <v>600</v>
@@ -13239,7 +13239,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="K119">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="L119">
         <v>600</v>
@@ -13283,7 +13283,7 @@
         <v>0.218</v>
       </c>
       <c r="K120">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="L120">
         <v>600</v>

</xml_diff>

<commit_message>
current state (new derivation)
</commit_message>
<xml_diff>
--- a/conejo/formatted_data.xlsx
+++ b/conejo/formatted_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\pyComms\conejo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6942DF3-E2AB-44A2-9EC7-8C7A84B76E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A92BF20-120E-47A7-A288-37703C701984}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="1455" windowWidth="14850" windowHeight="10200" activeTab="2" xr2:uid="{B2B3255C-86D4-4B94-9983-7EF4502B7862}"/>
+    <workbookView xWindow="8775" yWindow="2130" windowWidth="15720" windowHeight="12360" activeTab="1" xr2:uid="{B2B3255C-86D4-4B94-9983-7EF4502B7862}"/>
   </bookViews>
   <sheets>
     <sheet name="busses" sheetId="2" r:id="rId1"/>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FB4950-8AF2-4919-9162-03A3918F6395}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE3EA53-F01C-4E2B-BB06-AD151A3AC232}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="M68" sqref="M68:M101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5322,7 +5322,7 @@
         <v>34</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>1.0210999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -5363,7 +5363,7 @@
         <v>35</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>1.1254</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -5404,7 +5404,7 @@
         <v>36</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>1.1141000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -5445,7 +5445,7 @@
         <v>37</v>
       </c>
       <c r="M38">
-        <v>1</v>
+        <v>1.1016999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -5486,7 +5486,7 @@
         <v>38</v>
       </c>
       <c r="M39">
-        <v>1</v>
+        <v>1.0333000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -5527,7 +5527,7 @@
         <v>39</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>1.1564000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -5568,7 +5568,7 @@
         <v>40</v>
       </c>
       <c r="M41">
-        <v>1</v>
+        <v>1.1174999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -5609,7 +5609,7 @@
         <v>41</v>
       </c>
       <c r="M42">
-        <v>1</v>
+        <v>1.085</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -5650,7 +5650,7 @@
         <v>42</v>
       </c>
       <c r="M43">
-        <v>1</v>
+        <v>1.1011</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -5691,7 +5691,7 @@
         <v>43</v>
       </c>
       <c r="M44">
-        <v>1</v>
+        <v>1.0869</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -5732,7 +5732,7 @@
         <v>44</v>
       </c>
       <c r="M45">
-        <v>1</v>
+        <v>1.0125</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -5773,7 +5773,7 @@
         <v>45</v>
       </c>
       <c r="M46">
-        <v>1</v>
+        <v>1.0857000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -5814,7 +5814,7 @@
         <v>46</v>
       </c>
       <c r="M47">
-        <v>1</v>
+        <v>1.0584</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -5855,7 +5855,7 @@
         <v>47</v>
       </c>
       <c r="M48">
-        <v>1</v>
+        <v>1.0509999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -5896,7 +5896,7 @@
         <v>48</v>
       </c>
       <c r="M49">
-        <v>1</v>
+        <v>1.0422</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -5937,7 +5937,7 @@
         <v>49</v>
       </c>
       <c r="M50">
-        <v>1</v>
+        <v>1.0732999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -5978,7 +5978,7 @@
         <v>50</v>
       </c>
       <c r="M51">
-        <v>1</v>
+        <v>0.99990000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -6019,7 +6019,7 @@
         <v>51</v>
       </c>
       <c r="M52">
-        <v>1</v>
+        <v>1.1482000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -6060,7 +6060,7 @@
         <v>52</v>
       </c>
       <c r="M53">
-        <v>1</v>
+        <v>1.1259999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -6101,7 +6101,7 @@
         <v>53</v>
       </c>
       <c r="M54">
-        <v>1</v>
+        <v>1.099</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -6142,7 +6142,7 @@
         <v>54</v>
       </c>
       <c r="M55">
-        <v>1</v>
+        <v>1.0983000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -6183,7 +6183,7 @@
         <v>55</v>
       </c>
       <c r="M56">
-        <v>1</v>
+        <v>1.0601</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -6224,7 +6224,7 @@
         <v>56</v>
       </c>
       <c r="M57">
-        <v>1</v>
+        <v>1.1509</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -6265,7 +6265,7 @@
         <v>57</v>
       </c>
       <c r="M58">
-        <v>1</v>
+        <v>1.0932999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -6306,7 +6306,7 @@
         <v>58</v>
       </c>
       <c r="M59">
-        <v>1</v>
+        <v>1.0643</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -6347,7 +6347,7 @@
         <v>59</v>
       </c>
       <c r="M60">
-        <v>1</v>
+        <v>1.1676</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -6388,7 +6388,7 @@
         <v>60</v>
       </c>
       <c r="M61">
-        <v>1</v>
+        <v>1.0888</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -6429,7 +6429,7 @@
         <v>61</v>
       </c>
       <c r="M62">
-        <v>1</v>
+        <v>1.0705</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -6470,7 +6470,7 @@
         <v>62</v>
       </c>
       <c r="M63">
-        <v>1</v>
+        <v>1.0852999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -6511,7 +6511,7 @@
         <v>63</v>
       </c>
       <c r="M64">
-        <v>1</v>
+        <v>1.0576000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -6552,7 +6552,7 @@
         <v>64</v>
       </c>
       <c r="M65">
-        <v>1</v>
+        <v>1.044</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -6593,7 +6593,7 @@
         <v>65</v>
       </c>
       <c r="M66">
-        <v>1</v>
+        <v>1.2262999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -6634,7 +6634,7 @@
         <v>66</v>
       </c>
       <c r="M67">
-        <v>1</v>
+        <v>1.1828000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -6675,7 +6675,7 @@
         <v>67</v>
       </c>
       <c r="M68">
-        <v>1.0210999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -6716,7 +6716,7 @@
         <v>68</v>
       </c>
       <c r="M69">
-        <v>1.1254</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -6757,7 +6757,7 @@
         <v>69</v>
       </c>
       <c r="M70">
-        <v>1.1141000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -6798,7 +6798,7 @@
         <v>70</v>
       </c>
       <c r="M71">
-        <v>1.1016999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -6839,7 +6839,7 @@
         <v>71</v>
       </c>
       <c r="M72">
-        <v>1.0333000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -6880,7 +6880,7 @@
         <v>72</v>
       </c>
       <c r="M73">
-        <v>1.1564000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -6921,7 +6921,7 @@
         <v>73</v>
       </c>
       <c r="M74">
-        <v>1.1174999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>74</v>
       </c>
       <c r="M75">
-        <v>1.085</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -7003,7 +7003,7 @@
         <v>75</v>
       </c>
       <c r="M76">
-        <v>1.1011</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -7044,7 +7044,7 @@
         <v>76</v>
       </c>
       <c r="M77">
-        <v>1.0869</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -7085,7 +7085,7 @@
         <v>77</v>
       </c>
       <c r="M78">
-        <v>1.0125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -7126,7 +7126,7 @@
         <v>78</v>
       </c>
       <c r="M79">
-        <v>1.0857000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -7167,7 +7167,7 @@
         <v>79</v>
       </c>
       <c r="M80">
-        <v>1.0584</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -7208,7 +7208,7 @@
         <v>80</v>
       </c>
       <c r="M81">
-        <v>1.0509999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -7249,7 +7249,7 @@
         <v>81</v>
       </c>
       <c r="M82">
-        <v>1.0422</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -7290,7 +7290,7 @@
         <v>82</v>
       </c>
       <c r="M83">
-        <v>1.0732999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -7331,7 +7331,7 @@
         <v>83</v>
       </c>
       <c r="M84">
-        <v>0.99990000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -7372,7 +7372,7 @@
         <v>84</v>
       </c>
       <c r="M85">
-        <v>1.1482000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -7413,7 +7413,7 @@
         <v>85</v>
       </c>
       <c r="M86">
-        <v>1.1259999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -7454,7 +7454,7 @@
         <v>86</v>
       </c>
       <c r="M87">
-        <v>1.099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -7495,7 +7495,7 @@
         <v>87</v>
       </c>
       <c r="M88">
-        <v>1.0983000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -7536,7 +7536,7 @@
         <v>88</v>
       </c>
       <c r="M89">
-        <v>1.0601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -7577,7 +7577,7 @@
         <v>89</v>
       </c>
       <c r="M90">
-        <v>1.1509</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -7618,7 +7618,7 @@
         <v>90</v>
       </c>
       <c r="M91">
-        <v>1.0932999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -7659,7 +7659,7 @@
         <v>91</v>
       </c>
       <c r="M92">
-        <v>1.0643</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -7700,7 +7700,7 @@
         <v>92</v>
       </c>
       <c r="M93">
-        <v>1.1676</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -7741,7 +7741,7 @@
         <v>93</v>
       </c>
       <c r="M94">
-        <v>1.0888</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -7782,7 +7782,7 @@
         <v>94</v>
       </c>
       <c r="M95">
-        <v>1.0705</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -7823,7 +7823,7 @@
         <v>95</v>
       </c>
       <c r="M96">
-        <v>1.0852999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -7864,7 +7864,7 @@
         <v>96</v>
       </c>
       <c r="M97">
-        <v>1.0576000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -7905,7 +7905,7 @@
         <v>97</v>
       </c>
       <c r="M98">
-        <v>1.044</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -7946,7 +7946,7 @@
         <v>98</v>
       </c>
       <c r="M99">
-        <v>1.2262999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -7987,11 +7987,14 @@
         <v>99</v>
       </c>
       <c r="M100">
-        <v>1.1828000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
+      <c r="M101">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8005,8 +8008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F8381-333D-427E-B2F5-663E2125B366}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="K121" sqref="K121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>